<commit_message>
change product form and images upload
</commit_message>
<xml_diff>
--- a/public/2.xlsx
+++ b/public/2.xlsx
@@ -867,7 +867,7 @@
         <v>45127.910449887844</v>
       </c>
       <c r="K11" s="2">
-        <v>45127.91045099278</v>
+        <v>45283.62365946074</v>
       </c>
       <c r="L11" s="0" t="inlineStr">
         <is>
@@ -939,11 +939,11 @@
         <v>45127.911970067886</v>
       </c>
       <c r="K12" s="2">
-        <v>45269.852937876945</v>
+        <v>45282.824562320624</v>
       </c>
       <c r="L12" s="0" t="inlineStr">
         <is>
-          <t>http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBaVVCIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--865f62f348195c4c379bcc696a752bd8d60ae4b2/photo_2023-11-16_14-04-26.jpg http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBaWdCIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--e47e8c5eee04253249437cd597b1052ef03aaac8/20231206_144841.jpeg http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBaW9CIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--01a4fba5ccc9f6d098937b745405685674147955/20231206_144824.jpeg http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBaWtCIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--792961be0c0e408ac6c395c511a30195d8759a6c/20231206_144932.jpeg</t>
+          <t>http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBaVVCIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--865f62f348195c4c379bcc696a752bd8d60ae4b2/photo_2023-11-16_14-04-26.jpg http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBaWdCIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--e47e8c5eee04253249437cd597b1052ef03aaac8/20231206_144841.jpeg http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBaW9CIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--01a4fba5ccc9f6d098937b745405685674147955/20231206_144824.jpeg http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBaWtCIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--792961be0c0e408ac6c395c511a30195d8759a6c/20231206_144932.jpeg http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBbEFCIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--037d5e78e5747c3681fe52d3d42ce4b877178871/InSales%20API%20%F0%9F%94%8A%202023-08-17%2011-58-36.png</t>
         </is>
       </c>
       <c r="M12" s="0" t="inlineStr">

</xml_diff>

<commit_message>
add dashboard and fullsearch
</commit_message>
<xml_diff>
--- a/public/2.xlsx
+++ b/public/2.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showRuler="1" showWhiteSpace="0" showZeros="1" tabSelected="0" windowProtection="0" showOutlineSymbols="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -977,6 +977,150 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I13" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J13" s="2">
+        <v>45283.87358929602</v>
+      </c>
+      <c r="K13" s="2">
+        <v>45283.88173452872</v>
+      </c>
+      <c r="L13" s="0" t="inlineStr">
+        <is>
+          <t>http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBcFVEIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--fa7d7dcb19f78a8deb7ec8a7ba00f68ba73c2c0b/erp_fav.png http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBcGNEIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--034db0a4868dde326e1e9d8a47c66b5734f71fc3/Shopify%20Partners%202023-12-21%2019-38-52.png</t>
+        </is>
+      </c>
+      <c r="M13" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N13" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O13" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P13" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q13" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R13" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I14" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J14" s="2">
+        <v>45283.88737998698</v>
+      </c>
+      <c r="K14" s="2">
+        <v>45283.888460052156</v>
+      </c>
+      <c r="L14" s="0" t="inlineStr">
+        <is>
+          <t>http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBcG9EIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--732939eb1b2890b7bf2728c1621f14d7500d6e76/%D0%A2%D0%BE%D1%87%D0%BA%D0%B0%20%D0%A0%D0%BE%D1%81%D1%82%D0%B0%20-%20%D0%9F%D1%80%D0%BE%D0%B8%D0%B7%D0%B2%D0%BE%D0%BB%D1%8C%D0%BD%D1%8B%D0%B8%CC%86%20%D1%82%D0%BE%D0%B2%D0%B0%D1%80%20(vendor.model)%20-%20%D0%90%D0%B4%D0%B2%D0%B5%D0%BD%D1%82%D0%B5%D1%80%20-%20%D1%82%D0%BE%D0%B2%D0%B0%D1%80%D0%BD%D0%BE-%D0%BF%D1%80%D0%BE%D0%B8%D0%B7%D0%B2%D0%BE%D0%B4%D1%81%D1%82%D0%B2%D0%B5%D0%BD%D0%BD%D0%B0%D1%8F%20%D0%BA%D0%BE%D0%BC%D0%BF%D0%B0%D0%BD%D0%B8%D1%8F%20-%20InSales%202023-12-21%2012-14-53.png http://localhost:3000/rails/active_storage/blobs/redirect/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBcHdEIiwiZXhwIjpudWxsLCJwdXIiOiJibG9iX2lkIn19--1682b57df3e50da59010c87fc126b5ea3654ad7e/Gmail%202023-12-13%2012-21-05.png</t>
+        </is>
+      </c>
+      <c r="M14" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N14" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O14" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P14" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q14" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R14" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <printOptions gridLines="0" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>